<commit_message>
Added gloss to CombinationPlot
</commit_message>
<xml_diff>
--- a/CombinationPlot.xlsx
+++ b/CombinationPlot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biegertm\OneDrive - Starkey\Desktop\Toss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BFA1FBF-808F-4B2E-987B-E40945646860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462E766E-76E2-42BE-BD0D-564D4AA5459B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>FROM:</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Overlap</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>https://peltiertech.com/clustered-column-and-line-combination-chart/</t>
   </si>
 </sst>
 </file>
@@ -266,13 +272,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -382,7 +389,7 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
+  <tableStyles count="2" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
@@ -392,6 +399,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{1FB6757D-25C4-41EE-8122-64F7D4E79524}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1742,6 +1750,270 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>564510</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>114717</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Chart, box and whisker chart&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{834664CE-9701-F901-3C8E-FA8D24C8E69A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6812280" y="6202680"/>
+          <a:ext cx="7270110" cy="4808637"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>183477</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>137651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Chart&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F126A73-59B3-D881-5868-7040D7EF8614}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6812280" y="11399520"/>
+          <a:ext cx="6889077" cy="5669771"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>46305</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>122163</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Graphical user interface, text, application, email&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFB3CA77-CA57-EDD5-8D96-0C5DEBEC4765}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6812280" y="17266920"/>
+          <a:ext cx="6751905" cy="2804403"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>137753</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>122221</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Graphical user interface, text, application, email&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B56B2330-8524-295F-A362-3A87B5813214}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6812280" y="20284440"/>
+          <a:ext cx="6843353" cy="3475021"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>328270</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>160455</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Graphical user interface, application, table&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6494D394-AB9E-3730-D70C-500BDC75380F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6812280" y="23804880"/>
+          <a:ext cx="7033870" cy="5022015"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>152994</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>30584</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="Text&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91949C4B-0FD4-8A14-6DEB-1CF2508CCEFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6812280" y="29001720"/>
+          <a:ext cx="6858594" cy="1204064"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1993,11 +2265,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J175" sqref="J175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2024,6 +2299,14 @@
         <v>13-Sep-2021</v>
       </c>
       <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
@@ -2388,8 +2671,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{6517DC2D-60EC-445B-AFD5-591F96D44C84}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>